<commit_message>
minor changes in ExcelUtil and RemoteTests
</commit_message>
<xml_diff>
--- a/resources/RemoteTestData.xlsx
+++ b/resources/RemoteTestData.xlsx
@@ -17,28 +17,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="83">
   <si>
-    <t>50.01</t>
-  </si>
-  <si>
     <t>internet explorer</t>
   </si>
   <si>
     <t>Windows 7</t>
-  </si>
-  <si>
-    <t>30.01</t>
-  </si>
-  <si>
-    <t>50.02</t>
-  </si>
-  <si>
-    <t>30.02</t>
-  </si>
-  <si>
-    <t>50.03</t>
-  </si>
-  <si>
-    <t>30.03</t>
   </si>
   <si>
     <t>50.05</t>
@@ -223,15 +205,6 @@
     <t>Comment9</t>
   </si>
   <si>
-    <t>test1@test.com</t>
-  </si>
-  <si>
-    <t>test2@test.com</t>
-  </si>
-  <si>
-    <t>test3@test.com</t>
-  </si>
-  <si>
     <t>test5@test.com</t>
   </si>
   <si>
@@ -266,6 +239,33 @@
   </si>
   <si>
     <t>testLastName9</t>
+  </si>
+  <si>
+    <t>50.011</t>
+  </si>
+  <si>
+    <t>30.011</t>
+  </si>
+  <si>
+    <t>50.012</t>
+  </si>
+  <si>
+    <t>30.012</t>
+  </si>
+  <si>
+    <t>50.013</t>
+  </si>
+  <si>
+    <t>30.013</t>
+  </si>
+  <si>
+    <t>test11@test.com</t>
+  </si>
+  <si>
+    <t>test21@test.com</t>
+  </si>
+  <si>
+    <t>test31@test.com</t>
   </si>
 </sst>
 </file>
@@ -641,166 +641,166 @@
   <sheetData>
     <row r="1" spans="1:18" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="O3" s="1" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -822,218 +822,218 @@
   <sheetData>
     <row r="1" spans="1:18" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="R3" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remote Platforms without Robot changed
</commit_message>
<xml_diff>
--- a/resources/RemoteTestData.xlsx
+++ b/resources/RemoteTestData.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="temp" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="105">
   <si>
     <t>internet explorer</t>
   </si>
@@ -137,17 +137,9 @@
     <t>problemSolution9</t>
   </si>
   <si>
-    <t>http://i.imgur.com/HHXCVbs.jpg
-http://i.imgur.com/1K6AdCH.jpg</t>
-  </si>
-  <si>
     <t>http://i.imgur.com/1K6AdCH.jpg</t>
   </si>
   <si>
-    <t>imageComment1
-imageComment2</t>
-  </si>
-  <si>
     <t>imageComment1</t>
   </si>
   <si>
@@ -238,33 +230,6 @@
     <t>testLastName9</t>
   </si>
   <si>
-    <t>50.011</t>
-  </si>
-  <si>
-    <t>30.011</t>
-  </si>
-  <si>
-    <t>50.012</t>
-  </si>
-  <si>
-    <t>30.012</t>
-  </si>
-  <si>
-    <t>50.013</t>
-  </si>
-  <si>
-    <t>30.013</t>
-  </si>
-  <si>
-    <t>test11@test.com</t>
-  </si>
-  <si>
-    <t>test21@test.com</t>
-  </si>
-  <si>
-    <t>test31@test.com</t>
-  </si>
-  <si>
     <t>1</t>
   </si>
   <si>
@@ -319,7 +284,52 @@
     <t>#</t>
   </si>
   <si>
-    <t>WINDOWS</t>
+    <t>WIN8</t>
+  </si>
+  <si>
+    <t>MAC</t>
+  </si>
+  <si>
+    <t>50.0111</t>
+  </si>
+  <si>
+    <t>30.0111</t>
+  </si>
+  <si>
+    <t>50.0112</t>
+  </si>
+  <si>
+    <t>30.0112</t>
+  </si>
+  <si>
+    <t>50.0113</t>
+  </si>
+  <si>
+    <t>30.0113</t>
+  </si>
+  <si>
+    <t>50.0114</t>
+  </si>
+  <si>
+    <t>30.0114</t>
+  </si>
+  <si>
+    <t>50.0115</t>
+  </si>
+  <si>
+    <t>30.0115</t>
+  </si>
+  <si>
+    <t>50.0116</t>
+  </si>
+  <si>
+    <t>30.0116</t>
+  </si>
+  <si>
+    <t>50.0117</t>
+  </si>
+  <si>
+    <t>30.0117</t>
   </si>
 </sst>
 </file>
@@ -355,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -364,6 +374,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -667,9 +680,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -694,83 +709,83 @@
     <col min="20" max="16384" width="17" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>98</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -784,37 +799,41 @@
       <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="P2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q2" s="4" t="str">
+        <f>"test30" &amp; P2&amp; "@test.com"</f>
+        <v>test30testLastName1@test.com</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>48</v>
+      <c r="U2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="V2" s="4" t="str">
+        <f>"test30" &amp; U2&amp; "@test.com"</f>
+        <v>test301@test.com</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -823,13 +842,13 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>20</v>
@@ -843,37 +862,41 @@
       <c r="J3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="O3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3" s="4" t="str">
+        <f t="shared" ref="Q3:Q8" si="0">"test30" &amp; P3&amp; "@test.com"</f>
+        <v>test30testLastName2@test.com</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="S3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="V3" s="4" t="str">
+        <f t="shared" ref="V3:V8" si="1">"test30" &amp; U3&amp; "@test.com"</f>
+        <v>test302@test.com</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -882,13 +905,13 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -905,33 +928,290 @@
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>test30testLastName3@test.com</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="S4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="V4" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>test303@test.com</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O5" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q5" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>test30testLastName5@test.com</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="V5" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>test304@test.com</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="P6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="Q4" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>52</v>
+      <c r="Q6" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>test30testLastName6@test.com</v>
+      </c>
+      <c r="R6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="V6" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>test305@test.com</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q7" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>test30testLastName8@test.com</v>
+      </c>
+      <c r="R7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="U7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="V7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>test306@test.com</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q8" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>test30testLastName9@test.com</v>
+      </c>
+      <c r="R8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="V8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>test307@test.com</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="K3" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -939,7 +1219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:R4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -972,31 +1254,31 @@
         <v>33</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1030,25 +1312,25 @@
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="R2" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1080,31 +1362,31 @@
         <v>37</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="R3" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1138,25 +1420,25 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="M4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q4" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="R4" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SetVisibleView and ClickAtVisibleMapCenter methods added
</commit_message>
<xml_diff>
--- a/resources/RemoteTestData.xlsx
+++ b/resources/RemoteTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="112">
   <si>
     <t>internet explorer</t>
   </si>
@@ -330,6 +330,27 @@
   </si>
   <si>
     <t>30.0117</t>
+  </si>
+  <si>
+    <t>test401@test.com</t>
+  </si>
+  <si>
+    <t>test402@test.com</t>
+  </si>
+  <si>
+    <t>test403@test.com</t>
+  </si>
+  <si>
+    <t>test404@test.com</t>
+  </si>
+  <si>
+    <t>test405@test.com</t>
+  </si>
+  <si>
+    <t>test406@test.com</t>
+  </si>
+  <si>
+    <t>test407@test.com</t>
   </si>
 </sst>
 </file>
@@ -381,7 +402,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -394,9 +415,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -434,7 +455,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -506,7 +527,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -682,9 +703,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2:Q8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -697,8 +716,7 @@
     <col min="8" max="8" width="24" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17" style="1"/>
+    <col min="11" max="12" width="3" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -813,9 +831,8 @@
       <c r="P2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Q2" s="4" t="str">
-        <f>"test30" &amp; P2&amp; "@test.com"</f>
-        <v>test30testLastName1@test.com</v>
+      <c r="Q2" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>45</v>
@@ -827,8 +844,8 @@
         <v>71</v>
       </c>
       <c r="V2" s="4" t="str">
-        <f>"test30" &amp; U2&amp; "@test.com"</f>
-        <v>test301@test.com</v>
+        <f>"test40" &amp; U2&amp; "@test.com"</f>
+        <v>test401@test.com</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -876,9 +893,8 @@
       <c r="P3" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="Q3" s="4" t="str">
-        <f t="shared" ref="Q3:Q8" si="0">"test30" &amp; P3&amp; "@test.com"</f>
-        <v>test30testLastName2@test.com</v>
+      <c r="Q3" s="4" t="s">
+        <v>106</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>45</v>
@@ -890,8 +906,8 @@
         <v>72</v>
       </c>
       <c r="V3" s="4" t="str">
-        <f t="shared" ref="V3:V8" si="1">"test30" &amp; U3&amp; "@test.com"</f>
-        <v>test302@test.com</v>
+        <f t="shared" ref="V3:V8" si="0">"test40" &amp; U3&amp; "@test.com"</f>
+        <v>test402@test.com</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -939,9 +955,8 @@
       <c r="P4" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="Q4" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>test30testLastName3@test.com</v>
+      <c r="Q4" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>45</v>
@@ -953,8 +968,8 @@
         <v>73</v>
       </c>
       <c r="V4" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>test303@test.com</v>
+        <f t="shared" si="0"/>
+        <v>test403@test.com</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1002,9 +1017,8 @@
       <c r="P5" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="Q5" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>test30testLastName5@test.com</v>
+      <c r="Q5" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>45</v>
@@ -1016,8 +1030,8 @@
         <v>74</v>
       </c>
       <c r="V5" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>test304@test.com</v>
+        <f t="shared" si="0"/>
+        <v>test404@test.com</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -1065,9 +1079,8 @@
       <c r="P6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="Q6" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>test30testLastName6@test.com</v>
+      <c r="Q6" s="4" t="s">
+        <v>109</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>45</v>
@@ -1079,8 +1092,8 @@
         <v>75</v>
       </c>
       <c r="V6" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>test305@test.com</v>
+        <f t="shared" si="0"/>
+        <v>test405@test.com</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -1128,9 +1141,8 @@
       <c r="P7" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="Q7" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>test30testLastName8@test.com</v>
+      <c r="Q7" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="R7" s="3" t="s">
         <v>45</v>
@@ -1142,8 +1154,8 @@
         <v>76</v>
       </c>
       <c r="V7" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>test306@test.com</v>
+        <f t="shared" si="0"/>
+        <v>test406@test.com</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1191,9 +1203,8 @@
       <c r="P8" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="Q8" s="4" t="str">
-        <f t="shared" si="0"/>
-        <v>test30testLastName9@test.com</v>
+      <c r="Q8" s="4" t="s">
+        <v>111</v>
       </c>
       <c r="R8" s="3" t="s">
         <v>45</v>
@@ -1205,8 +1216,8 @@
         <v>77</v>
       </c>
       <c r="V8" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>test307@test.com</v>
+        <f t="shared" si="0"/>
+        <v>test407@test.com</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RemoteTestTwo and LocalTestThree added
</commit_message>
<xml_diff>
--- a/resources/RemoteTestData.xlsx
+++ b/resources/RemoteTestData.xlsx
@@ -290,67 +290,67 @@
     <t>MAC</t>
   </si>
   <si>
-    <t>50.0111</t>
-  </si>
-  <si>
-    <t>30.0111</t>
-  </si>
-  <si>
-    <t>50.0112</t>
-  </si>
-  <si>
-    <t>30.0112</t>
-  </si>
-  <si>
-    <t>50.0113</t>
-  </si>
-  <si>
-    <t>30.0113</t>
-  </si>
-  <si>
-    <t>50.0114</t>
-  </si>
-  <si>
-    <t>30.0114</t>
-  </si>
-  <si>
-    <t>50.0115</t>
-  </si>
-  <si>
-    <t>30.0115</t>
-  </si>
-  <si>
-    <t>50.0116</t>
-  </si>
-  <si>
-    <t>30.0116</t>
-  </si>
-  <si>
-    <t>50.0117</t>
-  </si>
-  <si>
-    <t>30.0117</t>
-  </si>
-  <si>
-    <t>test401@test.com</t>
-  </si>
-  <si>
-    <t>test402@test.com</t>
-  </si>
-  <si>
-    <t>test403@test.com</t>
-  </si>
-  <si>
-    <t>test404@test.com</t>
-  </si>
-  <si>
-    <t>test405@test.com</t>
-  </si>
-  <si>
-    <t>test406@test.com</t>
-  </si>
-  <si>
-    <t>test407@test.com</t>
+    <t>30.0511</t>
+  </si>
+  <si>
+    <t>50.0511</t>
+  </si>
+  <si>
+    <t>50.0512</t>
+  </si>
+  <si>
+    <t>30.0512</t>
+  </si>
+  <si>
+    <t>50.0513</t>
+  </si>
+  <si>
+    <t>30.0513</t>
+  </si>
+  <si>
+    <t>50.0514</t>
+  </si>
+  <si>
+    <t>30.0514</t>
+  </si>
+  <si>
+    <t>50.0515</t>
+  </si>
+  <si>
+    <t>30.0515</t>
+  </si>
+  <si>
+    <t>50.0516</t>
+  </si>
+  <si>
+    <t>30.0516</t>
+  </si>
+  <si>
+    <t>50.0517</t>
+  </si>
+  <si>
+    <t>30.0517</t>
+  </si>
+  <si>
+    <t>test701@test.com</t>
+  </si>
+  <si>
+    <t>test702@test.com</t>
+  </si>
+  <si>
+    <t>test703@test.com</t>
+  </si>
+  <si>
+    <t>test704@test.com</t>
+  </si>
+  <si>
+    <t>test705@test.com</t>
+  </si>
+  <si>
+    <t>test706@test.com</t>
+  </si>
+  <si>
+    <t>test707@test.com</t>
   </si>
 </sst>
 </file>
@@ -703,7 +703,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -800,10 +802,10 @@
         <v>89</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -844,8 +846,8 @@
         <v>71</v>
       </c>
       <c r="V2" s="4" t="str">
-        <f>"test40" &amp; U2&amp; "@test.com"</f>
-        <v>test401@test.com</v>
+        <f>"test70" &amp; U2&amp; "@test.com"</f>
+        <v>test701@test.com</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -906,8 +908,8 @@
         <v>72</v>
       </c>
       <c r="V3" s="4" t="str">
-        <f t="shared" ref="V3:V8" si="0">"test40" &amp; U3&amp; "@test.com"</f>
-        <v>test402@test.com</v>
+        <f t="shared" ref="V3:V8" si="0">"test70" &amp; U3&amp; "@test.com"</f>
+        <v>test702@test.com</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -969,7 +971,7 @@
       </c>
       <c r="V4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>test403@test.com</v>
+        <v>test703@test.com</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1031,7 +1033,7 @@
       </c>
       <c r="V5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>test404@test.com</v>
+        <v>test704@test.com</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
@@ -1093,7 +1095,7 @@
       </c>
       <c r="V6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>test405@test.com</v>
+        <v>test705@test.com</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -1155,7 +1157,7 @@
       </c>
       <c r="V7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>test406@test.com</v>
+        <v>test706@test.com</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1217,7 +1219,7 @@
       </c>
       <c r="V8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>test407@test.com</v>
+        <v>test707@test.com</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in Remote tests and Test data
</commit_message>
<xml_diff>
--- a/resources/RemoteTestData.xlsx
+++ b/resources/RemoteTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="120">
   <si>
     <t>internet explorer</t>
   </si>
@@ -149,24 +149,15 @@
     <t>admin</t>
   </si>
   <si>
-    <t>testFirstName1</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
     <t>Comment1</t>
   </si>
   <si>
-    <t>testFirstName2</t>
-  </si>
-  <si>
     <t>Comment2</t>
   </si>
   <si>
-    <t>testFirstName3</t>
-  </si>
-  <si>
     <t>Comment3</t>
   </si>
   <si>
@@ -209,15 +200,6 @@
     <t>9</t>
   </si>
   <si>
-    <t>testLastName1</t>
-  </si>
-  <si>
-    <t>testLastName2</t>
-  </si>
-  <si>
-    <t>testLastName3</t>
-  </si>
-  <si>
     <t>testLastName5</t>
   </si>
   <si>
@@ -290,67 +272,109 @@
     <t>MAC</t>
   </si>
   <si>
-    <t>30.0511</t>
-  </si>
-  <si>
-    <t>50.0511</t>
-  </si>
-  <si>
-    <t>50.0512</t>
-  </si>
-  <si>
-    <t>30.0512</t>
-  </si>
-  <si>
-    <t>50.0513</t>
-  </si>
-  <si>
-    <t>30.0513</t>
-  </si>
-  <si>
-    <t>50.0514</t>
-  </si>
-  <si>
-    <t>30.0514</t>
-  </si>
-  <si>
-    <t>50.0515</t>
-  </si>
-  <si>
-    <t>30.0515</t>
-  </si>
-  <si>
-    <t>50.0516</t>
-  </si>
-  <si>
-    <t>30.0516</t>
-  </si>
-  <si>
-    <t>50.0517</t>
-  </si>
-  <si>
-    <t>30.0517</t>
-  </si>
-  <si>
-    <t>test701@test.com</t>
-  </si>
-  <si>
-    <t>test702@test.com</t>
-  </si>
-  <si>
-    <t>test703@test.com</t>
-  </si>
-  <si>
-    <t>test704@test.com</t>
-  </si>
-  <si>
-    <t>test705@test.com</t>
-  </si>
-  <si>
-    <t>test706@test.com</t>
-  </si>
-  <si>
-    <t>test707@test.com</t>
+    <t>50.071</t>
+  </si>
+  <si>
+    <t>30.071</t>
+  </si>
+  <si>
+    <t>50.072</t>
+  </si>
+  <si>
+    <t>30.072</t>
+  </si>
+  <si>
+    <t>50.073</t>
+  </si>
+  <si>
+    <t>30.073</t>
+  </si>
+  <si>
+    <t>50.074</t>
+  </si>
+  <si>
+    <t>30.074</t>
+  </si>
+  <si>
+    <t>50.075</t>
+  </si>
+  <si>
+    <t>30.075</t>
+  </si>
+  <si>
+    <t>50.076</t>
+  </si>
+  <si>
+    <t>30.076</t>
+  </si>
+  <si>
+    <t>50.077</t>
+  </si>
+  <si>
+    <t>30.077</t>
+  </si>
+  <si>
+    <t>FirstName1</t>
+  </si>
+  <si>
+    <t>LastName1</t>
+  </si>
+  <si>
+    <t>FirstName2</t>
+  </si>
+  <si>
+    <t>LastName2</t>
+  </si>
+  <si>
+    <t>FirstName3</t>
+  </si>
+  <si>
+    <t>LastName3</t>
+  </si>
+  <si>
+    <t>FirstName4</t>
+  </si>
+  <si>
+    <t>LastName4</t>
+  </si>
+  <si>
+    <t>FirstName5</t>
+  </si>
+  <si>
+    <t>LastName5</t>
+  </si>
+  <si>
+    <t>FirstName6</t>
+  </si>
+  <si>
+    <t>LastName6</t>
+  </si>
+  <si>
+    <t>FirstName7</t>
+  </si>
+  <si>
+    <t>LastName7</t>
+  </si>
+  <si>
+    <t>test901@test.com</t>
+  </si>
+  <si>
+    <t>test902@test.com</t>
+  </si>
+  <si>
+    <t>test903@test.com</t>
+  </si>
+  <si>
+    <t>test904@test.com</t>
+  </si>
+  <si>
+    <t>test905@test.com</t>
+  </si>
+  <si>
+    <t>test906@test.com</t>
+  </si>
+  <si>
+    <t>test907@test.com</t>
   </si>
 </sst>
 </file>
@@ -402,7 +426,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -415,9 +439,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -455,7 +479,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -527,7 +551,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -703,7 +727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2:Q8"/>
     </sheetView>
   </sheetViews>
@@ -731,81 +755,81 @@
   <sheetData>
     <row r="1" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="J1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="K1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>14</v>
@@ -828,31 +852,31 @@
         <v>43</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="R2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="U2" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="V2" s="4" t="str">
-        <f>"test70" &amp; U2&amp; "@test.com"</f>
-        <v>test701@test.com</v>
+        <f>"test90" &amp; U2&amp; "@test.com"</f>
+        <v>test901@test.com</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -861,13 +885,13 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>20</v>
@@ -889,32 +913,32 @@
       <c r="N3" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>65</v>
+      <c r="O3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>102</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="V3" s="4" t="str">
-        <f t="shared" ref="V3:V8" si="0">"test70" &amp; U3&amp; "@test.com"</f>
-        <v>test702@test.com</v>
+        <f t="shared" ref="V3:V8" si="0">"test90" &amp; U3&amp; "@test.com"</f>
+        <v>test902@test.com</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -923,13 +947,13 @@
         <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="F4" s="3" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -951,32 +975,32 @@
       <c r="N4" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>66</v>
+      <c r="O4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>104</v>
       </c>
       <c r="Q4" s="4" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="V4" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>test703@test.com</v>
+        <v>test903@test.com</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -988,10 +1012,10 @@
         <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>22</v>
@@ -1014,31 +1038,31 @@
         <v>43</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>51</v>
+        <v>105</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="V5" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>test704@test.com</v>
+        <v>test904@test.com</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
@@ -1050,10 +1074,10 @@
         <v>12</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>23</v>
@@ -1076,31 +1100,31 @@
         <v>43</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>68</v>
+        <v>108</v>
       </c>
       <c r="Q6" s="4" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="V6" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>test705@test.com</v>
+        <v>test905@test.com</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>9</v>
@@ -1109,13 +1133,13 @@
         <v>10</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>24</v>
@@ -1138,31 +1162,31 @@
         <v>43</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>55</v>
+        <v>109</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>69</v>
+        <v>110</v>
       </c>
       <c r="Q7" s="4" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="V7" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>test706@test.com</v>
+        <v>test906@test.com</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
@@ -1171,13 +1195,13 @@
         <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>25</v>
@@ -1200,26 +1224,26 @@
         <v>43</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>57</v>
+        <v>111</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="Q8" s="4" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S8" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="V8" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>test707@test.com</v>
+        <v>test907@test.com</v>
       </c>
     </row>
   </sheetData>
@@ -1279,19 +1303,19 @@
         <v>43</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1331,19 +1355,19 @@
         <v>43</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
@@ -1387,19 +1411,19 @@
         <v>43</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1439,19 +1463,19 @@
         <v>43</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>